<commit_message>
+ read and write to the DB
</commit_message>
<xml_diff>
--- a/ConverterPy/dblist_full.xlsx
+++ b/ConverterPy/dblist_full.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NANLI_DEV\DDATOZiiPOS_Config\ConverterPy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nan_Dev\DDATOZiiPOS_Config\ConverterPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71FFD0D-222A-487E-BFD6-7B54AF3FE44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99058CC8-A14C-4FD5-9296-58F7969E9B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="1725" windowWidth="25515" windowHeight="13725" xr2:uid="{8C629834-DCE4-40C6-8641-352A07DED492}"/>
+    <workbookView xWindow="5445" yWindow="8415" windowWidth="21600" windowHeight="11385" xr2:uid="{8C629834-DCE4-40C6-8641-352A07DED492}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>dblist</t>
   </si>
@@ -43,12 +43,6 @@
   </si>
   <si>
     <t>03Okami_Wantirna</t>
-  </si>
-  <si>
-    <t>04Okami_Footscray</t>
-  </si>
-  <si>
-    <t>05Okami_Brunswick</t>
   </si>
   <si>
     <t>06Okami_Fairfield</t>
@@ -502,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5058723-EFDB-46D1-BC8A-48E6C31AEB4F}">
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:A37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,17 +569,17 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
@@ -696,16 +690,6 @@
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>